<commit_message>
group a and b ok
</commit_message>
<xml_diff>
--- a/bim_agent/tableConvert.com_A.xlsx
+++ b/bim_agent/tableConvert.com_A.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhuxueying/multi_agent/bim_agent/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCBEE6E1-F1F2-6F42-A3D0-2BDD74AF7847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C1C8215-58B8-E743-8B63-2EBA03F86615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6100" yWindow="760" windowWidth="22580" windowHeight="16180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7560" yWindow="760" windowWidth="26120" windowHeight="17180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="162">
   <si>
     <t>No.</t>
   </si>
@@ -252,9 +252,6 @@
   </si>
   <si>
     <t>PLUMBINGWALL</t>
-  </si>
-  <si>
-    <t>Plumbing wall</t>
   </si>
   <si>
     <t>Service wall</t>
@@ -482,13 +479,69 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>INTERIOR_FLOOR_SLAB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>GENERIC_ELEMENT</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>CURTAIN_WALL</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ROOF_SLAB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>✓</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>STAIR_LANDING</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>FOUNDATION_SLAB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>BALCONY</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>EXTERIOR_WALL</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>INTERIOR_WALL</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>SHEAR_WALL</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plumbing wall</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>INDOOR_PARKING</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>GENERAL_ROOM</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -540,6 +593,20 @@
       <family val="4"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00B050"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -561,7 +628,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -571,6 +638,12 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -914,10 +987,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.6640625" defaultRowHeight="15"/>
@@ -928,6 +1001,7 @@
     <col min="4" max="4" width="12.5" customWidth="1"/>
     <col min="5" max="5" width="24.83203125" customWidth="1"/>
     <col min="6" max="6" width="13.83203125" customWidth="1"/>
+    <col min="7" max="7" width="25.83203125" customWidth="1"/>
     <col min="10" max="10" width="28.83203125" customWidth="1"/>
     <col min="11" max="11" width="14.83203125" customWidth="1"/>
     <col min="12" max="12" width="22.1640625" customWidth="1"/>
@@ -950,10 +1024,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>145</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>146</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>5</v>
@@ -981,11 +1055,14 @@
       <c r="E2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F2">
-        <v>0.8</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>147</v>
+      <c r="F2" s="6">
+        <v>0.71</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>146</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>13</v>
@@ -1013,11 +1090,14 @@
       <c r="E3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F3">
-        <v>0.8</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>147</v>
+      <c r="F3" s="6">
+        <v>0.62</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>146</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>13</v>
@@ -1045,11 +1125,14 @@
       <c r="E4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F4">
-        <v>0.8</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>147</v>
+      <c r="F4" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>146</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>13</v>
@@ -1077,11 +1160,14 @@
       <c r="E5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F5">
-        <v>0.8</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>147</v>
+      <c r="F5" s="6">
+        <v>0.71</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>146</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>28</v>
@@ -1109,11 +1195,14 @@
       <c r="E6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F6">
-        <v>0.8</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>147</v>
+      <c r="F6" s="6">
+        <v>0.66</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>146</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>33</v>
@@ -1141,11 +1230,14 @@
       <c r="E7" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F7">
-        <v>0.8</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>147</v>
+      <c r="F7" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>146</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>38</v>
@@ -1173,11 +1265,14 @@
       <c r="E8" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F8">
-        <v>0.3</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>148</v>
+      <c r="F8" s="6">
+        <v>0.95</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>146</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>38</v>
@@ -1205,10 +1300,13 @@
       <c r="E9" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F9">
-        <v>0.7</v>
-      </c>
-      <c r="G9" s="4" t="s">
+      <c r="F9" s="6">
+        <v>0.91</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="H9" s="5" t="s">
         <v>147</v>
       </c>
       <c r="J9" s="3" t="s">
@@ -1237,11 +1335,14 @@
       <c r="E10" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F10">
-        <v>0.7</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>147</v>
+      <c r="F10" s="6">
+        <v>0.93</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>146</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>13</v>
@@ -1269,11 +1370,14 @@
       <c r="E11" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F11">
-        <v>0.7</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>147</v>
+      <c r="F11" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>146</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>13</v>
@@ -1301,10 +1405,13 @@
       <c r="E12" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F12">
-        <v>0.3</v>
-      </c>
-      <c r="G12" s="4" t="s">
+      <c r="F12" s="6">
+        <v>0.95</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="H12" s="5" t="s">
         <v>147</v>
       </c>
       <c r="J12" s="3" t="s">
@@ -1333,11 +1440,14 @@
       <c r="E13" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F13">
-        <v>0.3</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>147</v>
+      <c r="F13" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>146</v>
       </c>
       <c r="J13" s="3" t="s">
         <v>64</v>
@@ -1365,11 +1475,14 @@
       <c r="E14" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="F14">
-        <v>0.4</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>147</v>
+      <c r="F14" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>146</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>64</v>
@@ -1397,11 +1510,14 @@
       <c r="E15" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F15">
-        <v>0.27900000000000003</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>148</v>
+      <c r="F15" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>146</v>
       </c>
       <c r="J15" s="3" t="s">
         <v>64</v>
@@ -1427,13 +1543,16 @@
         <v>11</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="F16">
-        <v>0.27900000000000003</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>148</v>
+        <v>159</v>
+      </c>
+      <c r="F16" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>146</v>
       </c>
       <c r="J16" s="3" t="s">
         <v>64</v>
@@ -1442,289 +1561,316 @@
         <v>14</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="18">
       <c r="A17" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>77</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E17" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F17" s="6">
+        <v>0.65</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="J17" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="F17">
-        <v>0.8</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>79</v>
       </c>
       <c r="K17" s="3" t="s">
         <v>14</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="18">
       <c r="A18" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>82</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E18" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F18" s="7">
+        <v>0.42</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="J18" s="3" t="s">
         <v>83</v>
-      </c>
-      <c r="F18">
-        <v>0.8</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>84</v>
       </c>
       <c r="K18" s="3" t="s">
         <v>14</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="18">
       <c r="A19" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>87</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E19" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F19" s="7">
+        <v>0.33</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="J19" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="F19">
-        <v>0.8</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>89</v>
       </c>
       <c r="K19" s="3" t="s">
         <v>14</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="18">
       <c r="A20" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>92</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>93</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E20" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F20" s="7">
+        <v>0.42</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="J20" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="F20">
-        <v>0.8</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>95</v>
       </c>
       <c r="K20" s="3" t="s">
         <v>20</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="18">
       <c r="A21" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E21" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F21" s="7">
+        <v>0.33</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="J21" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="F21">
-        <v>0.8</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="J21" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="K21" s="3" t="s">
         <v>20</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="18">
       <c r="A22" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>104</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E22" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F22" s="7">
+        <v>0.33</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="J22" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="F22">
-        <v>0.8</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="J22" s="3" t="s">
-        <v>106</v>
       </c>
       <c r="K22" s="3" t="s">
         <v>14</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="18">
       <c r="A23" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>108</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>109</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="F23">
-        <v>0.8</v>
-      </c>
-      <c r="G23" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="F23" s="7">
+        <v>0.33</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="H23" s="5" t="s">
         <v>147</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K23" s="3" t="s">
         <v>14</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="18">
       <c r="A24" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="C24" s="3" t="s">
         <v>112</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>113</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E24" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F24" s="7">
+        <v>0.23</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="J24" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="F24">
-        <v>0.8</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="J24" s="3" t="s">
-        <v>115</v>
       </c>
       <c r="K24" s="3" t="s">
         <v>14</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="18">
       <c r="A25" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="C25" s="3" t="s">
         <v>118</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>119</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E25" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="F25" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="J25" s="3" t="s">
         <v>120</v>
-      </c>
-      <c r="F25">
-        <v>0.8</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="J25" s="3" t="s">
-        <v>121</v>
       </c>
       <c r="K25" s="3" t="s">
         <v>20</v>
@@ -1735,28 +1881,31 @@
     </row>
     <row r="26" spans="1:12" ht="18">
       <c r="A26" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>122</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>123</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="F26">
-        <v>0.8</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>147</v>
+        <v>123</v>
+      </c>
+      <c r="F26" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>146</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K26" s="3" t="s">
         <v>20</v>
@@ -1767,28 +1916,31 @@
     </row>
     <row r="27" spans="1:12" ht="18">
       <c r="A27" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>125</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>126</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="F27">
-        <v>0.8</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>147</v>
+        <v>126</v>
+      </c>
+      <c r="F27" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>152</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K27" s="3" t="s">
         <v>20</v>
@@ -1799,25 +1951,28 @@
     </row>
     <row r="28" spans="1:12" ht="18">
       <c r="A28" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="C28" s="3" t="s">
         <v>129</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>130</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F28">
-        <v>0.6</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>147</v>
+        <v>130</v>
+      </c>
+      <c r="F28" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>146</v>
       </c>
       <c r="J28" s="3" t="s">
         <v>28</v>
@@ -1826,29 +1981,32 @@
         <v>20</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="18">
       <c r="A29" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>133</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>134</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="F29">
-        <v>0.6</v>
-      </c>
-      <c r="G29" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="F29" s="7">
+        <v>0.33</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="H29" s="5" t="s">
         <v>147</v>
       </c>
       <c r="J29" s="3" t="s">
@@ -1858,30 +2016,33 @@
         <v>20</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="18">
       <c r="A30" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="C30" s="3" t="s">
         <v>138</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>139</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="F30">
-        <v>0.6</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>147</v>
+        <v>139</v>
+      </c>
+      <c r="F30" s="7">
+        <v>0.35</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>152</v>
       </c>
       <c r="J30" s="3" t="s">
         <v>28</v>
@@ -1890,30 +2051,33 @@
         <v>20</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="18">
       <c r="A31" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>141</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>142</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="F31">
-        <v>0.7</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>147</v>
+        <v>142</v>
+      </c>
+      <c r="F31" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>152</v>
       </c>
       <c r="J31" s="3" t="s">
         <v>28</v>
@@ -1922,8 +2086,13 @@
         <v>20</v>
       </c>
       <c r="L31" s="3" t="s">
-        <v>144</v>
-      </c>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="18">
+      <c r="F32" s="7"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>